<commit_message>
Update Wage ledger Report generator.
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/WageLegerReportTemplate.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/WageLegerReportTemplate.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,13 +9,16 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$O$45</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +55,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +109,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +144,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +352,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1"/>
+    <col min="3" max="15" width="10.7109375" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="74" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add header to WageLedgerReport.
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/WageLegerReportTemplate.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/WageLegerReportTemplate.xlsx
@@ -17,34 +17,31 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
-  <si>
-    <t>【部門】</t>
-  </si>
-  <si>
-    <t>【社員】</t>
-  </si>
-  <si>
-    <t>&amp;=HEADER.departmentCode</t>
-  </si>
-  <si>
-    <t>&amp;=HEADER.departmentName</t>
-  </si>
-  <si>
-    <t>&amp;=HEADER.employeeName</t>
-  </si>
-  <si>
-    <t>&amp;=HEADER.employeeCode</t>
-  </si>
-  <si>
-    <t>&amp;=HEADER.sex</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>DepartmentLabel</t>
+  </si>
+  <si>
+    <t>DepartmentInfo</t>
+  </si>
+  <si>
+    <t>EmployeeLabel</t>
+  </si>
+  <si>
+    <t>EmployeeInfo</t>
+  </si>
+  <si>
+    <t>SexLabel</t>
+  </si>
+  <si>
+    <t>SexInfo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,10 +51,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="IPAPGothic"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFA0A0A0"/>
-      <name val="Calibri"/>
+      <name val="IPAPGothic"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,16 +82,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,88 +408,80 @@
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="106" zoomScaleNormal="100" zoomScaleSheetLayoutView="106" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="2" customWidth="1"/>
-    <col min="21" max="21" width="9.140625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="4.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
+    <col min="3" max="15" width="10.7109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="2" style="1" customWidth="1"/>
+    <col min="17" max="20" width="9.140625" style="1"/>
+    <col min="21" max="21" width="9.140625" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T1" s="3"/>
-      <c r="U1" s="4" t="s">
+    <row r="1" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+    </row>
+    <row r="2" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+    </row>
+    <row r="3" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+    </row>
+    <row r="4" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="G4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-    </row>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T2" s="3"/>
-      <c r="U2" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-    </row>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T3" s="3"/>
-      <c r="U3" s="4" t="s">
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="L4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-    </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f>U1&amp;"    "&amp;U2</f>
-        <v>&amp;=HEADER.departmentCode    &amp;=HEADER.departmentName</v>
-      </c>
-      <c r="G4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" t="str">
-        <f>U3&amp;"       "&amp;U4</f>
-        <v>&amp;=HEADER.employeeName       &amp;=HEADER.employeeCode</v>
-      </c>
-      <c r="L4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M4" t="str">
-        <f>U5</f>
-        <v>&amp;=HEADER.sex</v>
-      </c>
-      <c r="T4" s="3"/>
-      <c r="U4" s="4" t="s">
+      <c r="M4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T5" s="3"/>
-      <c r="U5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
-      <c r="T6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
+      <c r="T4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+    </row>
+    <row r="5" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="W5" s="2"/>
+      <c r="X5" s="2"/>
+    </row>
+    <row r="6" spans="2:24" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="H4:J4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="73" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>

</xml_diff>